<commit_message>
renamed some stuff okay leaving now bai
</commit_message>
<xml_diff>
--- a/data/linkedin-data_techexpo15.xlsx
+++ b/data/linkedin-data_techexpo15.xlsx
@@ -1714,7 +1714,7 @@
   <dimension ref="A1:M64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2063,36 +2063,51 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>425</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>426</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>427</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>122</v>
+      </c>
+      <c r="F10">
+        <v>1993</v>
       </c>
       <c r="G10" t="s">
-        <v>81</v>
+        <v>428</v>
+      </c>
+      <c r="H10" t="s">
+        <v>429</v>
+      </c>
+      <c r="I10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10">
+        <v>60201</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
       </c>
       <c r="M10" t="s">
-        <v>82</v>
+        <v>430</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D11" t="s">
         <v>26</v>
@@ -2100,40 +2115,22 @@
       <c r="E11" t="s">
         <v>27</v>
       </c>
-      <c r="F11">
-        <v>2009</v>
-      </c>
       <c r="G11" t="s">
-        <v>86</v>
-      </c>
-      <c r="H11" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" t="s">
-        <v>88</v>
-      </c>
-      <c r="J11">
-        <v>92130</v>
-      </c>
-      <c r="K11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="M11" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
         <v>26</v>
@@ -2141,113 +2138,116 @@
       <c r="E12" t="s">
         <v>27</v>
       </c>
+      <c r="F12">
+        <v>2009</v>
+      </c>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H12" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="I12" t="s">
-        <v>96</v>
-      </c>
-      <c r="J12" t="s">
-        <v>97</v>
+        <v>88</v>
+      </c>
+      <c r="J12">
+        <v>92130</v>
       </c>
       <c r="K12" t="s">
         <v>21</v>
       </c>
       <c r="L12" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="M12" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="D13" t="s">
         <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13">
-        <v>1848</v>
+        <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H13" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="I13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13">
-        <v>60606</v>
+        <v>96</v>
+      </c>
+      <c r="J13" t="s">
+        <v>97</v>
       </c>
       <c r="K13" t="s">
         <v>21</v>
       </c>
       <c r="L13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="M13" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
         <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="F14">
-        <v>1871</v>
+        <v>1848</v>
       </c>
       <c r="G14" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H14" t="s">
-        <v>109</v>
-      </c>
-      <c r="J14" t="s">
-        <v>110</v>
+        <v>19</v>
+      </c>
+      <c r="I14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14">
+        <v>60606</v>
       </c>
       <c r="K14" t="s">
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="L14" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="M14" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
         <v>107</v>
@@ -2258,265 +2258,265 @@
       <c r="E15" t="s">
         <v>27</v>
       </c>
+      <c r="F15">
+        <v>1871</v>
+      </c>
       <c r="G15" t="s">
-        <v>116</v>
+        <v>108</v>
+      </c>
+      <c r="H15" t="s">
+        <v>109</v>
+      </c>
+      <c r="J15" t="s">
+        <v>110</v>
+      </c>
+      <c r="K15" t="s">
+        <v>111</v>
       </c>
       <c r="L15" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="M15" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>122</v>
-      </c>
-      <c r="F16">
-        <v>1996</v>
+        <v>27</v>
       </c>
       <c r="G16" t="s">
-        <v>123</v>
-      </c>
-      <c r="H16" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16">
-        <v>60614</v>
-      </c>
-      <c r="K16" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="L16" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="M16" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D17" t="s">
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="F17">
-        <v>1960</v>
+        <v>1996</v>
       </c>
       <c r="G17" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H17" t="s">
-        <v>130</v>
+        <v>19</v>
       </c>
       <c r="I17" t="s">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="J17">
-        <v>60018</v>
+        <v>60614</v>
       </c>
       <c r="K17" t="s">
         <v>21</v>
       </c>
+      <c r="L17" t="s">
+        <v>124</v>
+      </c>
       <c r="M17" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B18" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C18" t="s">
         <v>128</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
         <v>50</v>
       </c>
       <c r="F18">
-        <v>2005</v>
+        <v>1960</v>
       </c>
       <c r="G18" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H18" t="s">
-        <v>19</v>
+        <v>130</v>
       </c>
       <c r="I18" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="J18">
-        <v>60654</v>
+        <v>60018</v>
       </c>
       <c r="K18" t="s">
         <v>21</v>
       </c>
-      <c r="L18" t="s">
-        <v>136</v>
-      </c>
       <c r="M18" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
         <v>50</v>
       </c>
       <c r="F19">
-        <v>1988</v>
+        <v>2005</v>
       </c>
       <c r="G19" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="H19" t="s">
-        <v>142</v>
+        <v>19</v>
       </c>
       <c r="I19" t="s">
-        <v>143</v>
+        <v>20</v>
       </c>
       <c r="J19">
-        <v>20151</v>
+        <v>60654</v>
       </c>
       <c r="K19" t="s">
         <v>21</v>
       </c>
       <c r="L19" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="M19" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B20" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C20" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D20" t="s">
         <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>149</v>
+        <v>50</v>
       </c>
       <c r="F20">
-        <v>1979</v>
+        <v>1988</v>
       </c>
       <c r="G20" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="H20" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="I20" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="J20">
-        <v>53593</v>
+        <v>20151</v>
       </c>
       <c r="K20" t="s">
         <v>21</v>
       </c>
       <c r="L20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="M20" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B21" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>148</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>149</v>
+      </c>
+      <c r="F21">
+        <v>1979</v>
       </c>
       <c r="G21" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="H21" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="I21" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="J21">
-        <v>45242</v>
+        <v>53593</v>
       </c>
       <c r="K21" t="s">
         <v>21</v>
       </c>
       <c r="L21" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="M21" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B22" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C22" t="s">
-        <v>164</v>
+        <v>85</v>
       </c>
       <c r="D22" t="s">
         <v>26</v>
@@ -2524,332 +2524,317 @@
       <c r="E22" t="s">
         <v>50</v>
       </c>
-      <c r="F22">
-        <v>1912</v>
-      </c>
       <c r="G22" t="s">
-        <v>165</v>
+        <v>157</v>
+      </c>
+      <c r="H22" t="s">
+        <v>158</v>
+      </c>
+      <c r="I22" t="s">
+        <v>159</v>
+      </c>
+      <c r="J22">
+        <v>45242</v>
+      </c>
+      <c r="K22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" t="s">
+        <v>160</v>
       </c>
       <c r="M22" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B23" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C23" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D23" t="s">
         <v>26</v>
       </c>
       <c r="E23" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="F23">
+        <v>1912</v>
       </c>
       <c r="G23" t="s">
-        <v>170</v>
-      </c>
-      <c r="H23" t="s">
-        <v>158</v>
-      </c>
-      <c r="I23" t="s">
-        <v>159</v>
-      </c>
-      <c r="J23">
-        <v>45215</v>
-      </c>
-      <c r="K23" t="s">
-        <v>21</v>
-      </c>
-      <c r="L23" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="M23" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C24" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D24" t="s">
-        <v>176</v>
+        <v>26</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24">
-        <v>2002</v>
+        <v>27</v>
       </c>
       <c r="G24" t="s">
-        <v>177</v>
+        <v>170</v>
+      </c>
+      <c r="H24" t="s">
+        <v>158</v>
+      </c>
+      <c r="I24" t="s">
+        <v>159</v>
+      </c>
+      <c r="J24">
+        <v>45215</v>
+      </c>
+      <c r="K24" t="s">
+        <v>21</v>
       </c>
       <c r="L24" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="M24" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" t="s">
-        <v>180</v>
+        <v>414</v>
       </c>
       <c r="B25" t="s">
-        <v>181</v>
+        <v>415</v>
       </c>
       <c r="C25" t="s">
-        <v>140</v>
+        <v>416</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E25" t="s">
-        <v>182</v>
-      </c>
-      <c r="F25">
-        <v>1999</v>
+        <v>27</v>
       </c>
       <c r="G25" t="s">
-        <v>183</v>
-      </c>
-      <c r="H25" t="s">
-        <v>19</v>
-      </c>
-      <c r="I25" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25">
-        <v>60607</v>
-      </c>
-      <c r="K25" t="s">
-        <v>21</v>
+        <v>417</v>
       </c>
       <c r="L25" t="s">
-        <v>184</v>
+        <v>418</v>
       </c>
       <c r="M25" t="s">
-        <v>185</v>
+        <v>419</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="B26" t="s">
-        <v>181</v>
+        <v>361</v>
       </c>
       <c r="C26" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>182</v>
+        <v>27</v>
       </c>
       <c r="F26">
-        <v>1999</v>
+        <v>1898</v>
       </c>
       <c r="G26" t="s">
-        <v>183</v>
+        <v>362</v>
       </c>
       <c r="H26" t="s">
-        <v>19</v>
+        <v>363</v>
       </c>
       <c r="I26" t="s">
-        <v>20</v>
+        <v>159</v>
       </c>
       <c r="J26">
-        <v>60607</v>
+        <v>44316</v>
       </c>
       <c r="K26" t="s">
         <v>21</v>
       </c>
       <c r="L26" t="s">
-        <v>184</v>
+        <v>364</v>
       </c>
       <c r="M26" t="s">
-        <v>186</v>
+        <v>365</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="B27" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="C27" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="E27" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="F27">
-        <v>1985</v>
+        <v>2002</v>
       </c>
       <c r="G27" t="s">
-        <v>190</v>
-      </c>
-      <c r="H27" t="s">
-        <v>191</v>
-      </c>
-      <c r="I27" t="s">
-        <v>152</v>
-      </c>
-      <c r="J27">
-        <v>53188</v>
-      </c>
-      <c r="K27" t="s">
-        <v>21</v>
+        <v>177</v>
+      </c>
+      <c r="L27" t="s">
+        <v>178</v>
       </c>
       <c r="M27" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B28" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C28" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="D28" t="s">
         <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>182</v>
       </c>
       <c r="F28">
-        <v>1985</v>
+        <v>1999</v>
       </c>
       <c r="G28" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="H28" t="s">
-        <v>191</v>
+        <v>19</v>
       </c>
       <c r="I28" t="s">
-        <v>152</v>
+        <v>20</v>
       </c>
       <c r="J28">
-        <v>53188</v>
+        <v>60607</v>
       </c>
       <c r="K28" t="s">
         <v>21</v>
       </c>
+      <c r="L28" t="s">
+        <v>184</v>
+      </c>
       <c r="M28" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B29" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="C29" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="D29" t="s">
         <v>16</v>
       </c>
       <c r="E29" t="s">
-        <v>50</v>
+        <v>182</v>
       </c>
       <c r="F29">
-        <v>1985</v>
+        <v>1999</v>
       </c>
       <c r="G29" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="H29" t="s">
-        <v>197</v>
+        <v>19</v>
       </c>
       <c r="I29" t="s">
         <v>20</v>
       </c>
       <c r="J29">
-        <v>60069</v>
+        <v>60607</v>
       </c>
       <c r="K29" t="s">
         <v>21</v>
       </c>
       <c r="L29" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="M29" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="B30" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="C30" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="D30" t="s">
         <v>16</v>
       </c>
       <c r="E30" t="s">
-        <v>203</v>
+        <v>50</v>
       </c>
       <c r="F30">
-        <v>1989</v>
+        <v>1985</v>
       </c>
       <c r="G30" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="H30" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="I30" t="s">
-        <v>206</v>
-      </c>
-      <c r="J30" t="s">
-        <v>207</v>
+        <v>152</v>
+      </c>
+      <c r="J30">
+        <v>53188</v>
       </c>
       <c r="K30" t="s">
-        <v>208</v>
-      </c>
-      <c r="L30" t="s">
-        <v>209</v>
+        <v>21</v>
       </c>
       <c r="M30" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="B31" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>189</v>
       </c>
       <c r="D31" t="s">
         <v>16</v>
@@ -2858,118 +2843,118 @@
         <v>50</v>
       </c>
       <c r="F31">
-        <v>1961</v>
+        <v>1985</v>
       </c>
       <c r="G31" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="H31" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="I31" t="s">
-        <v>215</v>
+        <v>152</v>
       </c>
       <c r="J31">
-        <v>50309</v>
+        <v>53188</v>
       </c>
       <c r="K31" t="s">
         <v>21</v>
       </c>
       <c r="M31" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="B32" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
       <c r="C32" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="D32" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>149</v>
+        <v>50</v>
       </c>
       <c r="F32">
-        <v>1981</v>
+        <v>1985</v>
       </c>
       <c r="G32" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="H32" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="I32" t="s">
-        <v>222</v>
+        <v>20</v>
       </c>
       <c r="J32">
-        <v>5676</v>
+        <v>60069</v>
       </c>
       <c r="K32" t="s">
         <v>21</v>
       </c>
       <c r="L32" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="M32" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="B33" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
       <c r="C33" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="D33" t="s">
         <v>16</v>
       </c>
       <c r="E33" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
       <c r="F33">
-        <v>1884</v>
+        <v>1989</v>
       </c>
       <c r="G33" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="H33" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="I33" t="s">
-        <v>230</v>
-      </c>
-      <c r="J33">
-        <v>68131</v>
+        <v>206</v>
+      </c>
+      <c r="J33" t="s">
+        <v>207</v>
       </c>
       <c r="K33" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="L33" t="s">
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="M33" t="s">
-        <v>232</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
       <c r="B34" t="s">
-        <v>234</v>
+        <v>212</v>
       </c>
       <c r="C34" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="D34" t="s">
         <v>16</v>
@@ -2978,618 +2963,630 @@
         <v>50</v>
       </c>
       <c r="F34">
-        <v>1947</v>
+        <v>1961</v>
       </c>
       <c r="G34" t="s">
-        <v>235</v>
+        <v>213</v>
       </c>
       <c r="H34" t="s">
-        <v>236</v>
+        <v>214</v>
       </c>
       <c r="I34" t="s">
-        <v>237</v>
+        <v>215</v>
       </c>
       <c r="J34">
-        <v>1887</v>
+        <v>50309</v>
       </c>
       <c r="K34" t="s">
         <v>21</v>
       </c>
-      <c r="L34" t="s">
-        <v>238</v>
-      </c>
       <c r="M34" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="B35" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="C35" t="s">
-        <v>128</v>
+        <v>219</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E35" t="s">
-        <v>50</v>
+        <v>149</v>
       </c>
       <c r="F35">
-        <v>1901</v>
+        <v>1981</v>
       </c>
       <c r="G35" t="s">
-        <v>242</v>
+        <v>220</v>
       </c>
       <c r="H35" t="s">
-        <v>243</v>
+        <v>221</v>
       </c>
       <c r="I35" t="s">
-        <v>131</v>
+        <v>222</v>
       </c>
       <c r="J35">
-        <v>60126</v>
+        <v>5676</v>
       </c>
       <c r="K35" t="s">
         <v>21</v>
       </c>
       <c r="L35" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="M35" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="B36" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="C36" t="s">
-        <v>85</v>
+        <v>227</v>
       </c>
       <c r="D36" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E36" t="s">
         <v>27</v>
       </c>
       <c r="F36">
-        <v>1949</v>
+        <v>1884</v>
       </c>
       <c r="G36" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="H36" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="I36" t="s">
-        <v>250</v>
-      </c>
-      <c r="J36" t="s">
-        <v>251</v>
+        <v>230</v>
+      </c>
+      <c r="J36">
+        <v>68131</v>
       </c>
       <c r="K36" t="s">
         <v>21</v>
       </c>
       <c r="L36" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="M36" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="B37" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="C37" t="s">
-        <v>256</v>
+        <v>85</v>
       </c>
       <c r="D37" t="s">
-        <v>257</v>
+        <v>16</v>
       </c>
       <c r="E37" t="s">
-        <v>182</v>
+        <v>50</v>
       </c>
       <c r="F37">
-        <v>1999</v>
+        <v>1947</v>
       </c>
       <c r="G37" t="s">
-        <v>258</v>
+        <v>235</v>
+      </c>
+      <c r="H37" t="s">
+        <v>236</v>
+      </c>
+      <c r="I37" t="s">
+        <v>237</v>
+      </c>
+      <c r="J37">
+        <v>1887</v>
+      </c>
+      <c r="K37" t="s">
+        <v>21</v>
       </c>
       <c r="L37" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="M37" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="B38" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>128</v>
       </c>
       <c r="D38" t="s">
         <v>16</v>
       </c>
       <c r="E38" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="F38">
-        <v>2005</v>
+        <v>1901</v>
       </c>
       <c r="G38" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
       <c r="H38" t="s">
-        <v>19</v>
+        <v>243</v>
       </c>
       <c r="I38" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="J38">
-        <v>60634</v>
+        <v>60126</v>
       </c>
       <c r="K38" t="s">
         <v>21</v>
       </c>
       <c r="L38" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="M38" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="B39" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="C39" t="s">
-        <v>268</v>
+        <v>85</v>
       </c>
       <c r="D39" t="s">
         <v>26</v>
       </c>
       <c r="E39" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F39">
-        <v>1928</v>
+        <v>1949</v>
       </c>
       <c r="G39" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="H39" t="s">
-        <v>19</v>
+        <v>249</v>
       </c>
       <c r="I39" t="s">
-        <v>131</v>
-      </c>
-      <c r="J39">
-        <v>60654</v>
+        <v>250</v>
+      </c>
+      <c r="J39" t="s">
+        <v>251</v>
       </c>
       <c r="K39" t="s">
         <v>21</v>
       </c>
+      <c r="L39" t="s">
+        <v>252</v>
+      </c>
       <c r="M39" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="B40" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>256</v>
       </c>
       <c r="D40" t="s">
-        <v>16</v>
+        <v>257</v>
       </c>
       <c r="E40" t="s">
-        <v>149</v>
+        <v>182</v>
       </c>
       <c r="F40">
-        <v>1857</v>
+        <v>1999</v>
       </c>
       <c r="G40" t="s">
-        <v>273</v>
-      </c>
-      <c r="H40" t="s">
-        <v>274</v>
-      </c>
-      <c r="I40" t="s">
-        <v>152</v>
-      </c>
-      <c r="J40" t="s">
-        <v>275</v>
-      </c>
-      <c r="K40" t="s">
-        <v>21</v>
+        <v>258</v>
       </c>
       <c r="L40" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="M40" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="B41" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="C41" t="s">
-        <v>280</v>
+        <v>49</v>
       </c>
       <c r="D41" t="s">
-        <v>281</v>
+        <v>16</v>
       </c>
       <c r="E41" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="F41">
-        <v>1943</v>
+        <v>2005</v>
       </c>
       <c r="G41" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="H41" t="s">
-        <v>283</v>
+        <v>19</v>
       </c>
       <c r="I41" t="s">
-        <v>284</v>
+        <v>20</v>
       </c>
       <c r="J41">
-        <v>37831</v>
+        <v>60634</v>
       </c>
       <c r="K41" t="s">
         <v>21</v>
       </c>
       <c r="L41" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="M41" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="B42" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="C42" t="s">
-        <v>148</v>
+        <v>268</v>
       </c>
       <c r="D42" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E42" t="s">
-        <v>203</v>
+        <v>50</v>
       </c>
       <c r="F42">
-        <v>1980</v>
+        <v>1928</v>
       </c>
       <c r="G42" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="H42" t="s">
-        <v>290</v>
+        <v>19</v>
       </c>
       <c r="I42" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="J42">
-        <v>94577</v>
+        <v>60654</v>
       </c>
       <c r="K42" t="s">
         <v>21</v>
       </c>
-      <c r="L42" t="s">
-        <v>291</v>
-      </c>
       <c r="M42" t="s">
-        <v>292</v>
+        <v>270</v>
       </c>
     </row>
     <row r="43" spans="1:13">
       <c r="A43" t="s">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="B43" t="s">
-        <v>294</v>
+        <v>272</v>
       </c>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>15</v>
       </c>
       <c r="D43" t="s">
         <v>16</v>
       </c>
       <c r="E43" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="F43">
-        <v>1984</v>
+        <v>1857</v>
       </c>
       <c r="G43" t="s">
-        <v>295</v>
+        <v>273</v>
       </c>
       <c r="H43" t="s">
-        <v>296</v>
+        <v>274</v>
       </c>
       <c r="I43" t="s">
-        <v>297</v>
-      </c>
-      <c r="J43">
-        <v>3001</v>
+        <v>152</v>
+      </c>
+      <c r="J43" t="s">
+        <v>275</v>
       </c>
       <c r="K43" t="s">
-        <v>298</v>
+        <v>21</v>
       </c>
       <c r="L43" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
       <c r="M43" t="s">
-        <v>300</v>
+        <v>277</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" t="s">
-        <v>301</v>
+        <v>278</v>
       </c>
       <c r="B44" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
       <c r="C44" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="D44" t="s">
-        <v>26</v>
+        <v>281</v>
       </c>
       <c r="E44" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="F44">
+        <v>1943</v>
       </c>
       <c r="G44" t="s">
-        <v>304</v>
+        <v>282</v>
       </c>
       <c r="H44" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
       <c r="I44" t="s">
-        <v>306</v>
+        <v>284</v>
       </c>
       <c r="J44">
-        <v>10577</v>
+        <v>37831</v>
       </c>
       <c r="K44" t="s">
         <v>21</v>
       </c>
       <c r="L44" t="s">
-        <v>307</v>
+        <v>285</v>
       </c>
       <c r="M44" t="s">
-        <v>308</v>
+        <v>286</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="B45" t="s">
-        <v>310</v>
+        <v>288</v>
       </c>
       <c r="C45" t="s">
         <v>148</v>
       </c>
       <c r="D45" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E45" t="s">
-        <v>50</v>
+        <v>203</v>
       </c>
       <c r="F45">
-        <v>1985</v>
+        <v>1980</v>
       </c>
       <c r="G45" t="s">
-        <v>311</v>
+        <v>289</v>
       </c>
       <c r="H45" t="s">
-        <v>312</v>
+        <v>290</v>
       </c>
       <c r="I45" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="J45">
-        <v>77002</v>
+        <v>94577</v>
       </c>
       <c r="K45" t="s">
         <v>21</v>
       </c>
       <c r="L45" t="s">
-        <v>313</v>
+        <v>291</v>
       </c>
       <c r="M45" t="s">
-        <v>314</v>
+        <v>292</v>
       </c>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" t="s">
-        <v>315</v>
+        <v>293</v>
       </c>
       <c r="B46" t="s">
-        <v>316</v>
+        <v>294</v>
       </c>
       <c r="C46" t="s">
-        <v>317</v>
+        <v>121</v>
       </c>
       <c r="D46" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E46" t="s">
-        <v>27</v>
+        <v>122</v>
       </c>
       <c r="F46">
-        <v>1976</v>
+        <v>1984</v>
       </c>
       <c r="G46" t="s">
-        <v>318</v>
+        <v>295</v>
       </c>
       <c r="H46" t="s">
-        <v>319</v>
+        <v>296</v>
+      </c>
+      <c r="I46" t="s">
+        <v>297</v>
       </c>
       <c r="J46">
-        <v>11422</v>
+        <v>3001</v>
       </c>
       <c r="K46" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="L46" t="s">
-        <v>321</v>
+        <v>299</v>
       </c>
       <c r="M46" t="s">
-        <v>322</v>
+        <v>300</v>
       </c>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="B47" t="s">
-        <v>324</v>
+        <v>302</v>
       </c>
       <c r="C47" t="s">
-        <v>25</v>
+        <v>303</v>
       </c>
       <c r="D47" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E47" t="s">
-        <v>17</v>
-      </c>
-      <c r="F47">
-        <v>2010</v>
+        <v>27</v>
       </c>
       <c r="G47" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
       <c r="H47" t="s">
-        <v>19</v>
+        <v>305</v>
       </c>
       <c r="I47" t="s">
-        <v>131</v>
+        <v>306</v>
       </c>
       <c r="J47">
-        <v>60606</v>
+        <v>10577</v>
       </c>
       <c r="K47" t="s">
         <v>21</v>
       </c>
+      <c r="L47" t="s">
+        <v>307</v>
+      </c>
       <c r="M47" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="B48" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="C48" t="s">
-        <v>329</v>
+        <v>148</v>
       </c>
       <c r="D48" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E48" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="F48">
-        <v>1665</v>
+        <v>1985</v>
       </c>
       <c r="G48" t="s">
-        <v>330</v>
+        <v>311</v>
+      </c>
+      <c r="H48" t="s">
+        <v>312</v>
+      </c>
+      <c r="I48" t="s">
+        <v>96</v>
+      </c>
+      <c r="J48">
+        <v>77002</v>
+      </c>
+      <c r="K48" t="s">
+        <v>21</v>
       </c>
       <c r="L48" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="M48" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="B49" t="s">
-        <v>334</v>
+        <v>316</v>
       </c>
       <c r="C49" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="D49" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E49" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F49">
         <v>1976</v>
       </c>
       <c r="G49" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="H49" t="s">
-        <v>337</v>
-      </c>
-      <c r="I49" t="s">
-        <v>338</v>
+        <v>319</v>
       </c>
       <c r="J49">
-        <v>47151</v>
+        <v>11422</v>
       </c>
       <c r="K49" t="s">
-        <v>21</v>
+        <v>320</v>
       </c>
       <c r="L49" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="M49" t="s">
-        <v>340</v>
+        <v>322</v>
       </c>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="B50" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
       <c r="C50" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D50" t="s">
         <v>16</v>
@@ -3601,223 +3598,193 @@
         <v>2010</v>
       </c>
       <c r="G50" t="s">
-        <v>343</v>
+        <v>325</v>
+      </c>
+      <c r="H50" t="s">
+        <v>19</v>
+      </c>
+      <c r="I50" t="s">
+        <v>131</v>
+      </c>
+      <c r="J50">
+        <v>60606</v>
+      </c>
+      <c r="K50" t="s">
+        <v>21</v>
       </c>
       <c r="M50" t="s">
-        <v>344</v>
+        <v>326</v>
       </c>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" t="s">
-        <v>345</v>
+        <v>327</v>
       </c>
       <c r="B51" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
       <c r="C51" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="D51" t="s">
         <v>16</v>
       </c>
       <c r="E51" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F51">
-        <v>2007</v>
+        <v>1665</v>
       </c>
       <c r="G51" t="s">
-        <v>348</v>
-      </c>
-      <c r="H51" t="s">
-        <v>349</v>
-      </c>
-      <c r="I51" t="s">
-        <v>88</v>
-      </c>
-      <c r="J51">
-        <v>94040</v>
-      </c>
-      <c r="K51" t="s">
-        <v>21</v>
+        <v>330</v>
       </c>
       <c r="L51" t="s">
-        <v>350</v>
+        <v>331</v>
       </c>
       <c r="M51" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" t="s">
-        <v>352</v>
+        <v>333</v>
       </c>
       <c r="B52" t="s">
-        <v>353</v>
+        <v>334</v>
       </c>
       <c r="C52" t="s">
-        <v>25</v>
+        <v>335</v>
       </c>
       <c r="D52" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E52" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="F52">
-        <v>1968</v>
+        <v>1976</v>
       </c>
       <c r="G52" t="s">
-        <v>354</v>
+        <v>336</v>
       </c>
       <c r="H52" t="s">
-        <v>355</v>
+        <v>337</v>
       </c>
       <c r="I52" t="s">
-        <v>356</v>
+        <v>338</v>
       </c>
       <c r="J52">
-        <v>400001</v>
+        <v>47151</v>
       </c>
       <c r="K52" t="s">
-        <v>357</v>
+        <v>21</v>
       </c>
       <c r="L52" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="M52" t="s">
-        <v>359</v>
+        <v>340</v>
       </c>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" t="s">
-        <v>360</v>
+        <v>341</v>
       </c>
       <c r="B53" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
       <c r="C53" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E53" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F53">
-        <v>1898</v>
+        <v>2010</v>
       </c>
       <c r="G53" t="s">
-        <v>362</v>
-      </c>
-      <c r="H53" t="s">
-        <v>363</v>
-      </c>
-      <c r="I53" t="s">
-        <v>159</v>
-      </c>
-      <c r="J53">
-        <v>44316</v>
-      </c>
-      <c r="K53" t="s">
-        <v>21</v>
-      </c>
-      <c r="L53" t="s">
-        <v>364</v>
+        <v>343</v>
       </c>
       <c r="M53" t="s">
-        <v>365</v>
+        <v>344</v>
       </c>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
       <c r="B54" t="s">
-        <v>367</v>
+        <v>346</v>
       </c>
       <c r="C54" t="s">
-        <v>148</v>
+        <v>347</v>
       </c>
       <c r="D54" t="s">
         <v>16</v>
       </c>
       <c r="E54" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="F54">
-        <v>1984</v>
+        <v>2007</v>
       </c>
       <c r="G54" t="s">
-        <v>368</v>
+        <v>348</v>
       </c>
       <c r="H54" t="s">
-        <v>369</v>
+        <v>349</v>
       </c>
       <c r="I54" t="s">
-        <v>370</v>
+        <v>88</v>
       </c>
       <c r="J54">
-        <v>1760</v>
+        <v>94040</v>
       </c>
       <c r="K54" t="s">
         <v>21</v>
       </c>
+      <c r="L54" t="s">
+        <v>350</v>
+      </c>
       <c r="M54" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" t="s">
-        <v>372</v>
+        <v>420</v>
       </c>
       <c r="B55" t="s">
-        <v>373</v>
+        <v>421</v>
       </c>
       <c r="C55" t="s">
-        <v>189</v>
+        <v>422</v>
       </c>
       <c r="D55" t="s">
-        <v>16</v>
+        <v>281</v>
       </c>
       <c r="E55" t="s">
-        <v>203</v>
-      </c>
-      <c r="F55">
-        <v>1921</v>
+        <v>27</v>
       </c>
       <c r="G55" t="s">
-        <v>374</v>
-      </c>
-      <c r="H55" t="s">
-        <v>274</v>
-      </c>
-      <c r="I55" t="s">
-        <v>375</v>
-      </c>
-      <c r="J55">
-        <v>53219</v>
-      </c>
-      <c r="K55" t="s">
-        <v>21</v>
-      </c>
-      <c r="L55" t="s">
-        <v>376</v>
+        <v>423</v>
       </c>
       <c r="M55" t="s">
-        <v>377</v>
+        <v>424</v>
       </c>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" t="s">
-        <v>378</v>
+        <v>352</v>
       </c>
       <c r="B56" t="s">
-        <v>379</v>
+        <v>353</v>
       </c>
       <c r="C56" t="s">
-        <v>169</v>
+        <v>25</v>
       </c>
       <c r="D56" t="s">
         <v>26</v>
@@ -3825,119 +3792,119 @@
       <c r="E56" t="s">
         <v>27</v>
       </c>
+      <c r="F56">
+        <v>1968</v>
+      </c>
       <c r="G56" t="s">
-        <v>380</v>
+        <v>354</v>
       </c>
       <c r="H56" t="s">
-        <v>19</v>
+        <v>355</v>
       </c>
       <c r="I56" t="s">
-        <v>20</v>
+        <v>356</v>
       </c>
       <c r="J56">
-        <v>60606</v>
+        <v>400001</v>
       </c>
       <c r="K56" t="s">
-        <v>21</v>
+        <v>357</v>
       </c>
       <c r="L56" t="s">
-        <v>381</v>
+        <v>358</v>
       </c>
       <c r="M56" t="s">
-        <v>382</v>
+        <v>359</v>
       </c>
     </row>
     <row r="57" spans="1:13">
       <c r="A57" t="s">
-        <v>383</v>
+        <v>366</v>
       </c>
       <c r="B57" t="s">
-        <v>384</v>
+        <v>367</v>
       </c>
       <c r="C57" t="s">
-        <v>385</v>
+        <v>148</v>
       </c>
       <c r="D57" t="s">
-        <v>281</v>
+        <v>16</v>
       </c>
       <c r="E57" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="F57">
-        <v>1775</v>
+        <v>1984</v>
       </c>
       <c r="G57" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="H57" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="I57" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
       <c r="J57">
-        <v>20350</v>
+        <v>1760</v>
       </c>
       <c r="K57" t="s">
         <v>21</v>
       </c>
-      <c r="L57" t="s">
-        <v>389</v>
-      </c>
       <c r="M57" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
     </row>
     <row r="58" spans="1:13">
       <c r="A58" t="s">
-        <v>391</v>
+        <v>372</v>
       </c>
       <c r="B58" t="s">
-        <v>392</v>
+        <v>373</v>
       </c>
       <c r="C58" t="s">
-        <v>93</v>
+        <v>189</v>
       </c>
       <c r="D58" t="s">
         <v>16</v>
       </c>
       <c r="E58" t="s">
-        <v>182</v>
+        <v>203</v>
       </c>
       <c r="F58">
-        <v>1992</v>
+        <v>1921</v>
       </c>
       <c r="G58" t="s">
-        <v>393</v>
+        <v>374</v>
       </c>
       <c r="H58" t="s">
-        <v>394</v>
+        <v>274</v>
       </c>
       <c r="I58" t="s">
-        <v>20</v>
+        <v>375</v>
       </c>
       <c r="J58">
-        <v>60148</v>
+        <v>53219</v>
       </c>
       <c r="K58" t="s">
         <v>21</v>
       </c>
       <c r="L58" t="s">
-        <v>395</v>
+        <v>376</v>
       </c>
       <c r="M58" t="s">
-        <v>396</v>
+        <v>377</v>
       </c>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" t="s">
-        <v>397</v>
+        <v>378</v>
       </c>
       <c r="B59" t="s">
-        <v>398</v>
+        <v>379</v>
       </c>
       <c r="C59" t="s">
-        <v>399</v>
+        <v>169</v>
       </c>
       <c r="D59" t="s">
         <v>26</v>
@@ -3946,88 +3913,118 @@
         <v>27</v>
       </c>
       <c r="G59" t="s">
-        <v>400</v>
+        <v>380</v>
+      </c>
+      <c r="H59" t="s">
+        <v>19</v>
+      </c>
+      <c r="I59" t="s">
+        <v>20</v>
+      </c>
+      <c r="J59">
+        <v>60606</v>
+      </c>
+      <c r="K59" t="s">
+        <v>21</v>
       </c>
       <c r="L59" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="M59" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="B60" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="C60" t="s">
-        <v>202</v>
+        <v>385</v>
       </c>
       <c r="D60" t="s">
-        <v>16</v>
+        <v>281</v>
       </c>
       <c r="E60" t="s">
-        <v>182</v>
+        <v>27</v>
       </c>
       <c r="F60">
-        <v>2007</v>
+        <v>1775</v>
       </c>
       <c r="G60" t="s">
-        <v>405</v>
+        <v>386</v>
       </c>
       <c r="H60" t="s">
-        <v>406</v>
+        <v>387</v>
       </c>
       <c r="I60" t="s">
-        <v>407</v>
+        <v>388</v>
       </c>
       <c r="J60">
-        <v>6870</v>
+        <v>20350</v>
       </c>
       <c r="K60" t="s">
         <v>21</v>
       </c>
+      <c r="L60" t="s">
+        <v>389</v>
+      </c>
       <c r="M60" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
       <c r="B61" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
       <c r="C61" t="s">
-        <v>219</v>
+        <v>93</v>
       </c>
       <c r="D61" t="s">
         <v>16</v>
       </c>
       <c r="E61" t="s">
-        <v>27</v>
+        <v>182</v>
+      </c>
+      <c r="F61">
+        <v>1992</v>
       </c>
       <c r="G61" t="s">
-        <v>411</v>
+        <v>393</v>
+      </c>
+      <c r="H61" t="s">
+        <v>394</v>
+      </c>
+      <c r="I61" t="s">
+        <v>20</v>
+      </c>
+      <c r="J61">
+        <v>60148</v>
+      </c>
+      <c r="K61" t="s">
+        <v>21</v>
       </c>
       <c r="L61" t="s">
-        <v>412</v>
+        <v>395</v>
       </c>
       <c r="M61" t="s">
-        <v>413</v>
+        <v>396</v>
       </c>
     </row>
     <row r="62" spans="1:13">
       <c r="A62" t="s">
-        <v>414</v>
+        <v>397</v>
       </c>
       <c r="B62" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="C62" t="s">
-        <v>416</v>
+        <v>399</v>
       </c>
       <c r="D62" t="s">
         <v>26</v>
@@ -4036,77 +4033,83 @@
         <v>27</v>
       </c>
       <c r="G62" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="L62" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="M62" t="s">
-        <v>419</v>
+        <v>402</v>
       </c>
     </row>
     <row r="63" spans="1:13">
       <c r="A63" t="s">
-        <v>420</v>
+        <v>403</v>
       </c>
       <c r="B63" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
       <c r="C63" t="s">
-        <v>422</v>
+        <v>202</v>
       </c>
       <c r="D63" t="s">
-        <v>281</v>
+        <v>16</v>
       </c>
       <c r="E63" t="s">
-        <v>27</v>
+        <v>182</v>
+      </c>
+      <c r="F63">
+        <v>2007</v>
       </c>
       <c r="G63" t="s">
-        <v>423</v>
+        <v>405</v>
+      </c>
+      <c r="H63" t="s">
+        <v>406</v>
+      </c>
+      <c r="I63" t="s">
+        <v>407</v>
+      </c>
+      <c r="J63">
+        <v>6870</v>
+      </c>
+      <c r="K63" t="s">
+        <v>21</v>
       </c>
       <c r="M63" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
     </row>
     <row r="64" spans="1:13">
       <c r="A64" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="B64" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
       <c r="C64" t="s">
-        <v>427</v>
+        <v>219</v>
       </c>
       <c r="D64" t="s">
         <v>16</v>
       </c>
       <c r="E64" t="s">
-        <v>122</v>
-      </c>
-      <c r="F64">
-        <v>1993</v>
+        <v>27</v>
       </c>
       <c r="G64" t="s">
-        <v>428</v>
-      </c>
-      <c r="H64" t="s">
-        <v>429</v>
-      </c>
-      <c r="I64" t="s">
-        <v>20</v>
-      </c>
-      <c r="J64">
-        <v>60201</v>
-      </c>
-      <c r="K64" t="s">
-        <v>21</v>
+        <v>411</v>
+      </c>
+      <c r="L64" t="s">
+        <v>412</v>
       </c>
       <c r="M64" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:M64">
+    <sortCondition ref="A2:A64"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>